<commit_message>
GoodInfo_v2 - 2021.12.03 未完成
</commit_message>
<xml_diff>
--- a/GoodInfo_StockList_20211202.xlsx
+++ b/GoodInfo_StockList_20211202.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaeon365-my.sharepoint.com/personal/raywu_aaeon_com_tw/Documents/_OLD/Documents/Python/GoodInfo_v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{30137E35-B895-497D-9BBA-A9B428F7A711}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10572"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10572" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="96">
   <si>
     <t>名稱</t>
   </si>
@@ -40,9 +41,6 @@
   </si>
   <si>
     <t>券資比5日增減</t>
-  </si>
-  <si>
-    <t>一年最高股價_y</t>
   </si>
   <si>
     <t>大量_1</t>
@@ -318,7 +316,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -683,24 +681,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -721,10 +719,10 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>8</v>
@@ -747,19 +745,16 @@
       <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
       <c r="D2">
         <v>69.7</v>
@@ -783,36 +778,33 @@
         <v>9.99</v>
       </c>
       <c r="K2">
-        <v>69.099999999999994</v>
+        <v>4</v>
       </c>
       <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="M2">
         <v>4.53</v>
       </c>
-      <c r="O2">
+      <c r="N2">
         <v>2.95</v>
       </c>
-      <c r="R2" t="s">
-        <v>21</v>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2">
+        <v>5</v>
       </c>
       <c r="S2">
         <v>5</v>
       </c>
-      <c r="T2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
       <c r="D3">
         <v>57.8</v>
@@ -836,30 +828,27 @@
         <v>0.47</v>
       </c>
       <c r="K3">
-        <v>57.8</v>
-      </c>
-      <c r="L3">
         <v>4</v>
       </c>
-      <c r="R3" t="s">
-        <v>21</v>
+      <c r="Q3" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
       </c>
       <c r="D4">
         <v>25.45</v>
@@ -883,36 +872,33 @@
         <v>0.85</v>
       </c>
       <c r="K4">
-        <v>25.45</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4">
         <v>8.91</v>
       </c>
-      <c r="O4">
+      <c r="N4">
         <v>0</v>
       </c>
-      <c r="R4" t="s">
-        <v>21</v>
+      <c r="Q4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4">
+        <v>-3</v>
       </c>
       <c r="S4">
         <v>-3</v>
       </c>
-      <c r="T4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
       </c>
       <c r="D5">
         <v>293.5</v>
@@ -936,33 +922,30 @@
         <v>-6.06</v>
       </c>
       <c r="K5">
-        <v>293.5</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5">
         <v>1.72</v>
       </c>
-      <c r="R5" t="s">
-        <v>21</v>
+      <c r="Q5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>-1</v>
       </c>
       <c r="S5">
         <v>-1</v>
       </c>
-      <c r="T5">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
       </c>
       <c r="D6">
         <v>154</v>
@@ -986,36 +969,33 @@
         <v>-3.32</v>
       </c>
       <c r="K6">
-        <v>154</v>
+        <v>3</v>
       </c>
       <c r="L6">
+        <v>5.4</v>
+      </c>
+      <c r="N6">
+        <v>4.68</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6">
+        <v>-1</v>
+      </c>
+      <c r="S6">
         <v>3</v>
       </c>
-      <c r="M6">
-        <v>5.4</v>
-      </c>
-      <c r="O6">
-        <v>4.68</v>
-      </c>
-      <c r="R6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6">
-        <v>-1</v>
-      </c>
-      <c r="T6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
       </c>
       <c r="D7">
         <v>229.5</v>
@@ -1039,36 +1019,33 @@
         <v>-0.26</v>
       </c>
       <c r="K7">
-        <v>229.5</v>
+        <v>3</v>
       </c>
       <c r="L7">
-        <v>3</v>
-      </c>
-      <c r="M7">
         <v>2.33</v>
       </c>
-      <c r="O7">
+      <c r="N7">
         <v>6.22</v>
       </c>
-      <c r="R7" t="s">
-        <v>21</v>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <v>-3</v>
       </c>
       <c r="S7">
-        <v>-3</v>
-      </c>
-      <c r="T7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
       </c>
       <c r="D8">
         <v>266</v>
@@ -1092,36 +1069,33 @@
         <v>2.25</v>
       </c>
       <c r="K8">
-        <v>266</v>
+        <v>3</v>
       </c>
       <c r="L8">
-        <v>3</v>
-      </c>
-      <c r="M8">
         <v>6.71</v>
       </c>
-      <c r="O8">
+      <c r="N8">
         <v>5.97</v>
       </c>
-      <c r="R8" t="s">
-        <v>21</v>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
       </c>
       <c r="S8">
         <v>5</v>
       </c>
-      <c r="T8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
         <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
       </c>
       <c r="D9">
         <v>447.5</v>
@@ -1145,33 +1119,30 @@
         <v>4.79</v>
       </c>
       <c r="K9">
-        <v>447.5</v>
+        <v>3</v>
       </c>
       <c r="L9">
-        <v>3</v>
-      </c>
-      <c r="M9">
         <v>6.07</v>
       </c>
-      <c r="R9" t="s">
-        <v>21</v>
+      <c r="Q9" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
       </c>
       <c r="S9">
         <v>5</v>
       </c>
-      <c r="T9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>23</v>
       </c>
       <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -1195,30 +1166,27 @@
         <v>-2.4900000000000002</v>
       </c>
       <c r="K10">
-        <v>60</v>
-      </c>
-      <c r="L10">
         <v>3</v>
       </c>
-      <c r="R10" t="s">
-        <v>21</v>
+      <c r="Q10" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10">
+        <v>-1</v>
       </c>
       <c r="S10">
         <v>-1</v>
       </c>
-      <c r="T10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
         <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
       </c>
       <c r="D11">
         <v>278.5</v>
@@ -1242,36 +1210,33 @@
         <v>-2.2599999999999998</v>
       </c>
       <c r="K11">
-        <v>278.5</v>
+        <v>3</v>
       </c>
       <c r="L11">
-        <v>3</v>
-      </c>
-      <c r="M11">
         <v>4.46</v>
       </c>
-      <c r="O11">
+      <c r="N11">
         <v>3.32</v>
       </c>
-      <c r="R11" t="s">
-        <v>21</v>
+      <c r="Q11" t="s">
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>-5</v>
       </c>
       <c r="S11">
-        <v>-5</v>
-      </c>
-      <c r="T11">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>26</v>
       </c>
       <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
       </c>
       <c r="D12">
         <v>88.4</v>
@@ -1295,36 +1260,33 @@
         <v>2.66</v>
       </c>
       <c r="K12">
-        <v>88.4</v>
+        <v>3</v>
       </c>
       <c r="L12">
+        <v>3.65</v>
+      </c>
+      <c r="N12">
+        <v>12.26</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12">
         <v>3</v>
       </c>
-      <c r="M12">
-        <v>3.65</v>
-      </c>
-      <c r="O12">
-        <v>12.26</v>
-      </c>
-      <c r="R12" t="s">
-        <v>21</v>
-      </c>
       <c r="S12">
-        <v>3</v>
-      </c>
-      <c r="T12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>38</v>
       </c>
       <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
         <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>93</v>
       </c>
       <c r="D13">
         <v>73</v>
@@ -1348,30 +1310,27 @@
         <v>3.32</v>
       </c>
       <c r="K13">
-        <v>69.3</v>
-      </c>
-      <c r="L13">
         <v>3</v>
       </c>
-      <c r="R13" t="s">
-        <v>21</v>
+      <c r="Q13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
       </c>
       <c r="S13">
         <v>1</v>
       </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
       </c>
       <c r="D14">
         <v>283.5</v>
@@ -1395,30 +1354,27 @@
         <v>-1.82</v>
       </c>
       <c r="K14">
-        <v>283.5</v>
-      </c>
-      <c r="L14">
         <v>2.9</v>
       </c>
-      <c r="R14" t="s">
-        <v>21</v>
+      <c r="Q14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
       </c>
       <c r="S14">
-        <v>1</v>
-      </c>
-      <c r="T14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>24</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
       </c>
       <c r="D15">
         <v>204.5</v>
@@ -1442,30 +1398,27 @@
         <v>-0.32</v>
       </c>
       <c r="K15">
-        <v>204.5</v>
-      </c>
-      <c r="L15">
         <v>2.9</v>
       </c>
-      <c r="R15" t="s">
-        <v>21</v>
+      <c r="Q15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <v>-1</v>
       </c>
       <c r="S15">
         <v>-1</v>
       </c>
-      <c r="T15">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>35</v>
       </c>
       <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" t="s">
         <v>86</v>
-      </c>
-      <c r="C16" t="s">
-        <v>87</v>
       </c>
       <c r="D16">
         <v>631</v>
@@ -1489,30 +1442,27 @@
         <v>0.27</v>
       </c>
       <c r="K16">
-        <v>631</v>
-      </c>
-      <c r="L16">
         <v>2.9</v>
       </c>
-      <c r="R16" t="s">
-        <v>21</v>
+      <c r="Q16" t="s">
+        <v>20</v>
+      </c>
+      <c r="R16">
+        <v>-1</v>
       </c>
       <c r="S16">
-        <v>-1</v>
-      </c>
-      <c r="T16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>36</v>
       </c>
       <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
         <v>88</v>
-      </c>
-      <c r="C17" t="s">
-        <v>89</v>
       </c>
       <c r="D17">
         <v>131</v>
@@ -1536,36 +1486,33 @@
         <v>-1.1200000000000001</v>
       </c>
       <c r="K17">
-        <v>131</v>
+        <v>2.9</v>
       </c>
       <c r="L17">
-        <v>2.9</v>
-      </c>
-      <c r="M17">
         <v>0.72</v>
       </c>
-      <c r="O17">
+      <c r="N17">
         <v>6.7</v>
       </c>
-      <c r="R17" t="s">
-        <v>21</v>
+      <c r="Q17" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <v>-1</v>
       </c>
       <c r="S17">
         <v>-1</v>
       </c>
-      <c r="T17">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
         <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
       </c>
       <c r="D18">
         <v>73.2</v>
@@ -1589,30 +1536,27 @@
         <v>0.12</v>
       </c>
       <c r="K18">
-        <v>73.2</v>
-      </c>
-      <c r="L18">
         <v>2.8</v>
       </c>
-      <c r="R18" t="s">
-        <v>21</v>
+      <c r="Q18" t="s">
+        <v>20</v>
+      </c>
+      <c r="R18">
+        <v>-3</v>
       </c>
       <c r="S18">
         <v>-3</v>
       </c>
-      <c r="T18">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>7</v>
       </c>
       <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
       </c>
       <c r="D19">
         <v>148</v>
@@ -1636,30 +1580,27 @@
         <v>-0.47</v>
       </c>
       <c r="K19">
-        <v>148</v>
-      </c>
-      <c r="L19">
         <v>2.8</v>
       </c>
-      <c r="R19" t="s">
-        <v>21</v>
+      <c r="Q19" t="s">
+        <v>20</v>
+      </c>
+      <c r="R19">
+        <v>-1</v>
       </c>
       <c r="S19">
         <v>-1</v>
       </c>
-      <c r="T19">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>12</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="D20">
         <v>92.3</v>
@@ -1683,30 +1624,27 @@
         <v>0.09</v>
       </c>
       <c r="K20">
-        <v>92.3</v>
-      </c>
-      <c r="L20">
         <v>2.8</v>
       </c>
-      <c r="R20" t="s">
-        <v>21</v>
+      <c r="Q20" t="s">
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
       </c>
       <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>17</v>
       </c>
       <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" t="s">
-        <v>51</v>
       </c>
       <c r="D21">
         <v>260.5</v>
@@ -1730,30 +1668,27 @@
         <v>1.66</v>
       </c>
       <c r="K21">
-        <v>260.5</v>
-      </c>
-      <c r="L21">
         <v>2.8</v>
       </c>
-      <c r="R21" t="s">
-        <v>21</v>
+      <c r="Q21" t="s">
+        <v>20</v>
+      </c>
+      <c r="R21">
+        <v>5</v>
       </c>
       <c r="S21">
         <v>5</v>
       </c>
-      <c r="T21">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>28</v>
       </c>
       <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
         <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
       </c>
       <c r="D22">
         <v>165</v>
@@ -1777,30 +1712,27 @@
         <v>1.33</v>
       </c>
       <c r="K22">
-        <v>165</v>
-      </c>
-      <c r="L22">
         <v>2.8</v>
       </c>
-      <c r="R22" t="s">
-        <v>21</v>
+      <c r="Q22" t="s">
+        <v>20</v>
+      </c>
+      <c r="R22">
+        <v>5</v>
       </c>
       <c r="S22">
         <v>5</v>
       </c>
-      <c r="T22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>33</v>
       </c>
       <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
         <v>82</v>
-      </c>
-      <c r="C23" t="s">
-        <v>83</v>
       </c>
       <c r="D23">
         <v>323.5</v>
@@ -1824,30 +1756,27 @@
         <v>3.54</v>
       </c>
       <c r="K23">
-        <v>323.5</v>
-      </c>
-      <c r="L23">
         <v>2.8</v>
       </c>
-      <c r="R23" t="s">
-        <v>21</v>
+      <c r="Q23" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
       </c>
       <c r="S23">
         <v>1</v>
       </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>30</v>
       </c>
       <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
         <v>76</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
       </c>
       <c r="D24">
         <v>26</v>
@@ -1871,30 +1800,27 @@
         <v>3.3</v>
       </c>
       <c r="K24">
-        <v>24.6</v>
-      </c>
-      <c r="L24">
         <v>2.5</v>
       </c>
-      <c r="R24" t="s">
-        <v>21</v>
+      <c r="Q24" t="s">
+        <v>20</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
       </c>
       <c r="S24">
         <v>1</v>
       </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>34</v>
       </c>
       <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
         <v>84</v>
-      </c>
-      <c r="C25" t="s">
-        <v>85</v>
       </c>
       <c r="D25">
         <v>20.7</v>
@@ -1918,30 +1844,27 @@
         <v>-1.02</v>
       </c>
       <c r="K25">
-        <v>20.7</v>
-      </c>
-      <c r="L25">
         <v>2.5</v>
       </c>
-      <c r="R25" t="s">
-        <v>21</v>
+      <c r="Q25" t="s">
+        <v>20</v>
+      </c>
+      <c r="R25">
+        <v>5</v>
       </c>
       <c r="S25">
-        <v>5</v>
-      </c>
-      <c r="T25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>37</v>
       </c>
       <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
       </c>
       <c r="D26">
         <v>58.7</v>
@@ -1959,30 +1882,27 @@
         <v>-2.0299999999999998</v>
       </c>
       <c r="K26">
-        <v>58.7</v>
-      </c>
-      <c r="L26">
         <v>2.5</v>
       </c>
-      <c r="R26" t="s">
-        <v>21</v>
+      <c r="Q26" t="s">
+        <v>20</v>
+      </c>
+      <c r="R26">
+        <v>-4</v>
       </c>
       <c r="S26">
         <v>-4</v>
       </c>
-      <c r="T26">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>31</v>
       </c>
       <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
       <c r="D27">
         <v>71</v>
@@ -2006,30 +1926,27 @@
         <v>5.53</v>
       </c>
       <c r="K27">
-        <v>64.599999999999994</v>
-      </c>
-      <c r="L27">
         <v>2.4</v>
       </c>
-      <c r="R27" t="s">
-        <v>21</v>
+      <c r="Q27" t="s">
+        <v>20</v>
+      </c>
+      <c r="R27">
+        <v>5</v>
       </c>
       <c r="S27">
         <v>5</v>
       </c>
-      <c r="T27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>10</v>
       </c>
       <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
         <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>37</v>
       </c>
       <c r="D28">
         <v>44.6</v>
@@ -2053,30 +1970,27 @@
         <v>-0.15</v>
       </c>
       <c r="K28">
-        <v>44.6</v>
-      </c>
-      <c r="L28">
         <v>2</v>
       </c>
-      <c r="R28" t="s">
-        <v>21</v>
+      <c r="Q28" t="s">
+        <v>20</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
       </c>
       <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="T28">
         <v>-5</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>22</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
         <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
       </c>
       <c r="D29">
         <v>225</v>
@@ -2100,30 +2014,27 @@
         <v>0.25</v>
       </c>
       <c r="K29">
-        <v>225</v>
-      </c>
-      <c r="L29">
         <v>2</v>
       </c>
-      <c r="R29" t="s">
-        <v>21</v>
+      <c r="Q29" t="s">
+        <v>20</v>
+      </c>
+      <c r="R29">
+        <v>-1</v>
       </c>
       <c r="S29">
-        <v>-1</v>
-      </c>
-      <c r="T29">
         <v>-3</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
       </c>
       <c r="D30">
         <v>41</v>
@@ -2147,30 +2058,27 @@
         <v>0.08</v>
       </c>
       <c r="K30">
-        <v>41</v>
-      </c>
-      <c r="L30">
         <v>2</v>
       </c>
-      <c r="R30" t="s">
-        <v>21</v>
+      <c r="Q30" t="s">
+        <v>20</v>
+      </c>
+      <c r="R30">
+        <v>5</v>
       </c>
       <c r="S30">
-        <v>5</v>
-      </c>
-      <c r="T30">
         <v>-3</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
         <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>18</v>
       </c>
       <c r="D31">
         <v>93.1</v>
@@ -2193,25 +2101,25 @@
       <c r="J31">
         <v>-0.71</v>
       </c>
-      <c r="R31" t="s">
-        <v>16</v>
+      <c r="Q31" t="s">
+        <v>15</v>
+      </c>
+      <c r="R31">
+        <v>-1</v>
       </c>
       <c r="S31">
-        <v>-1</v>
-      </c>
-      <c r="T31">
         <v>-5</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
         <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>20</v>
       </c>
       <c r="D32">
         <v>25.95</v>
@@ -2234,28 +2142,25 @@
       <c r="J32">
         <v>5.13</v>
       </c>
-      <c r="K32">
-        <v>25.95</v>
-      </c>
-      <c r="R32" t="s">
-        <v>21</v>
+      <c r="Q32" t="s">
+        <v>20</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
       </c>
       <c r="S32">
         <v>1</v>
       </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>3</v>
       </c>
       <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
         <v>22</v>
-      </c>
-      <c r="C33" t="s">
-        <v>23</v>
       </c>
       <c r="D33">
         <v>16.55</v>
@@ -2278,28 +2183,25 @@
       <c r="J33">
         <v>4.6500000000000004</v>
       </c>
-      <c r="K33">
-        <v>16.55</v>
-      </c>
-      <c r="R33" t="s">
-        <v>21</v>
+      <c r="Q33" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
       </c>
       <c r="S33">
         <v>1</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>5</v>
       </c>
       <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
         <v>26</v>
-      </c>
-      <c r="C34" t="s">
-        <v>27</v>
       </c>
       <c r="D34">
         <v>72</v>
@@ -2322,28 +2224,25 @@
       <c r="J34">
         <v>0.72</v>
       </c>
-      <c r="K34">
-        <v>72</v>
-      </c>
-      <c r="R34" t="s">
-        <v>21</v>
+      <c r="Q34" t="s">
+        <v>20</v>
+      </c>
+      <c r="R34">
+        <v>5</v>
       </c>
       <c r="S34">
         <v>5</v>
       </c>
-      <c r="T34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>13</v>
       </c>
       <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
         <v>42</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
       </c>
       <c r="D35">
         <v>32.700000000000003</v>
@@ -2366,28 +2265,25 @@
       <c r="J35">
         <v>0.01</v>
       </c>
-      <c r="K35">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="R35" t="s">
-        <v>21</v>
+      <c r="Q35" t="s">
+        <v>20</v>
+      </c>
+      <c r="R35">
+        <v>3</v>
       </c>
       <c r="S35">
-        <v>3</v>
-      </c>
-      <c r="T35">
         <v>-3</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>16</v>
       </c>
       <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
         <v>48</v>
-      </c>
-      <c r="C36" t="s">
-        <v>49</v>
       </c>
       <c r="D36">
         <v>34.799999999999997</v>
@@ -2410,28 +2306,25 @@
       <c r="J36">
         <v>3.79</v>
       </c>
-      <c r="K36">
-        <v>33.25</v>
-      </c>
-      <c r="R36" t="s">
-        <v>21</v>
+      <c r="Q36" t="s">
+        <v>20</v>
+      </c>
+      <c r="R36">
+        <v>5</v>
       </c>
       <c r="S36">
         <v>5</v>
       </c>
-      <c r="T36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>20</v>
       </c>
       <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
         <v>56</v>
-      </c>
-      <c r="C37" t="s">
-        <v>57</v>
       </c>
       <c r="D37">
         <v>2240</v>
@@ -2454,28 +2347,25 @@
       <c r="J37">
         <v>3.11</v>
       </c>
-      <c r="K37">
-        <v>2240</v>
-      </c>
-      <c r="R37" t="s">
-        <v>21</v>
+      <c r="Q37" t="s">
+        <v>20</v>
+      </c>
+      <c r="R37">
+        <v>-1</v>
       </c>
       <c r="S37">
-        <v>-1</v>
-      </c>
-      <c r="T37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>21</v>
       </c>
       <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
         <v>58</v>
-      </c>
-      <c r="C38" t="s">
-        <v>59</v>
       </c>
       <c r="D38">
         <v>177</v>
@@ -2498,28 +2388,28 @@
       <c r="J38">
         <v>3.18</v>
       </c>
-      <c r="L38">
+      <c r="K38">
         <v>2.5</v>
       </c>
-      <c r="R38" t="s">
-        <v>16</v>
+      <c r="Q38" t="s">
+        <v>15</v>
+      </c>
+      <c r="R38">
+        <v>5</v>
       </c>
       <c r="S38">
         <v>5</v>
       </c>
-      <c r="T38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>32</v>
       </c>
       <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
         <v>80</v>
-      </c>
-      <c r="C39" t="s">
-        <v>81</v>
       </c>
       <c r="D39">
         <v>17.899999999999999</v>
@@ -2542,25 +2432,293 @@
       <c r="J39">
         <v>-2.71</v>
       </c>
-      <c r="L39">
+      <c r="K39">
         <v>2.5</v>
       </c>
-      <c r="R39" t="s">
-        <v>16</v>
+      <c r="Q39" t="s">
+        <v>15</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
       </c>
       <c r="S39">
         <v>1</v>
       </c>
-      <c r="T39">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:T39">
-    <sortCondition descending="1" ref="L1"/>
+  <sortState ref="A2:S39">
+    <sortCondition descending="1" ref="K1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068154D9CED6A274799344D73CDDB6092" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d5a2665e4f307efafdee1c9405c7148c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0" xmlns:ns4="a05e4abd-8455-4909-9372-067b8b6e3dbc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb69d6d218e7dc1efa9607e3a9562cb6" ns3:_="" ns4:_="">
+    <xsd:import namespace="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <xsd:import namespace="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:description="" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a05e4abd-8455-4909-9372-067b8b6e3dbc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C42725CA-1976-4F93-8CE1-198BCDAE0FD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CC2F6F8-5C4F-4610-9379-E69BD991B0D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40826C3C-F52E-484F-B194-3FD3E0216A91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="4bb3d3d4-acd0-4d8e-ae87-a4aef309b0b0"/>
+    <ds:schemaRef ds:uri="a05e4abd-8455-4909-9372-067b8b6e3dbc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>